<commit_message>
Fix files download bug
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_8_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_8_2022.xlsx
@@ -429,16 +429,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>800/PV FES 1</v>
+        <v>456/CASA</v>
       </c>
       <c r="B2" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>P5874857</v>
+        <v>BK747A53</v>
       </c>
       <c r="D2" t="str">
-        <v>KARIM JALAL</v>
+        <v>ANAS MASTI</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -447,45 +447,45 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>15</v>
-      </c>
-      <c r="H2" t="str">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1000</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="str">
         <v>--</v>
       </c>
-      <c r="I2">
-        <v>40000</v>
-      </c>
-      <c r="J2" t="str">
-        <v>--</v>
-      </c>
-      <c r="K2">
-        <v>6000</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>10000</v>
-      </c>
       <c r="O2">
-        <v>44000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve">044/LF/FES VILLE </v>
+        <v>456/CASA</v>
       </c>
       <c r="B3" t="str">
-        <v>Logement de fonction</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>L3578354</v>
+        <v>BG746583</v>
       </c>
       <c r="D3" t="str">
-        <v>NABIL KAMAL</v>
+        <v>TEST KAMAL</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -494,16 +494,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -518,21 +518,21 @@
         <v>--</v>
       </c>
       <c r="O3">
-        <v>8500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v xml:space="preserve">044/FES VILLE </v>
+        <v>456/CASA</v>
       </c>
       <c r="B4" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>K5443645</v>
+        <v>GT744635</v>
       </c>
       <c r="D4" t="str">
-        <v>KHADIJA LALA</v>
+        <v>JAMAL JAMAL</v>
       </c>
       <c r="E4" t="str">
         <v>non</v>
@@ -541,16 +541,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -565,7 +565,7 @@
         <v>--</v>
       </c>
       <c r="O4">
-        <v>8500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
@@ -591,28 +591,28 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="H5">
-        <v>20000</v>
+        <v>3000</v>
       </c>
       <c r="I5">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>3000</v>
-      </c>
-      <c r="K5">
-        <v>6000</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>10000</v>
-      </c>
-      <c r="O5">
-        <v>61000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>